<commit_message>
Remove 530 duplicate rows
</commit_message>
<xml_diff>
--- a/input_xlsx/RN_2018-09-21 (revisi).xlsx
+++ b/input_xlsx/RN_2018-09-21 (revisi).xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TAMBORA MUDA\DATA BIODIVERSKRIPSI\2018-09-21\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="6860" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Events" sheetId="2" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="Literature" sheetId="6" r:id="rId3"/>
     <sheet name="Measurement" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +28,7 @@
     <author>Primadieta</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -121,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -165,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -209,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -253,7 +248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -297,7 +292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -341,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -385,7 +380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -429,7 +424,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -473,7 +468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -517,7 +512,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -561,7 +556,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -605,7 +600,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -649,7 +644,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -693,7 +688,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -737,7 +732,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -781,7 +776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -825,7 +820,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0">
+    <comment ref="S1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -869,7 +864,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="1" shapeId="0">
+    <comment ref="U1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -904,7 +899,7 @@
     <author>Primadieta</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -948,7 +943,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -992,7 +987,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1036,7 +1031,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1080,7 +1075,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1124,7 +1119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1178,7 +1173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1222,7 +1217,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1266,7 +1261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1310,7 +1305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1354,7 +1349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1398,7 +1393,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1442,7 +1437,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1486,7 +1481,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1530,7 +1525,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1574,7 +1569,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1618,7 +1613,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1" shapeId="0">
+    <comment ref="Q1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1653,7 +1648,7 @@
     <author>Primadieta</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1697,7 +1692,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1741,7 +1736,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1785,7 +1780,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1829,7 +1824,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1873,7 +1868,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1917,7 +1912,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1961,7 +1956,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2005,7 +2000,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2049,7 +2044,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="1" shapeId="0">
+    <comment ref="J1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2083,7 +2078,7 @@
     <author>Kyle Braak</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2127,7 +2122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2171,7 +2166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2196,7 +2191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2240,7 +2235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2284,7 +2279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2328,7 +2323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2372,7 +2367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2416,7 +2411,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2465,7 +2460,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="322">
   <si>
     <t>occurrenceID</t>
   </si>
@@ -3142,24 +3137,6 @@
     <t>IPB-2000WN-RN001-SCIKk-VE005</t>
   </si>
   <si>
-    <t>IPB-2000WN-RN001-SCIKk-VE006</t>
-  </si>
-  <si>
-    <t>IPB-2000WN-RN001-SCIKk-VE007</t>
-  </si>
-  <si>
-    <t>IPB-2000WN-RN001-SCIKk-VE008</t>
-  </si>
-  <si>
-    <t>IPB-2000WN-RN001-SCIKk-VE009</t>
-  </si>
-  <si>
-    <t>IPB-2000WN-RN001-SCIKk-VE010</t>
-  </si>
-  <si>
-    <t>IPB-2000WN-RN001-SCIKk-VE011</t>
-  </si>
-  <si>
     <t>IPB-2000WN-RN001-SCISk-VE001</t>
   </si>
   <si>
@@ -3172,15 +3149,6 @@
     <t>IPB-2000WN-RN001-SCISk-VE004</t>
   </si>
   <si>
-    <t>IPB-2000WN-RN001-SCISk-VE005</t>
-  </si>
-  <si>
-    <t>IPB-2000WN-RN001-SCISk-VE006</t>
-  </si>
-  <si>
-    <t>IPB-2000WN-RN001-SCISk-VE007</t>
-  </si>
-  <si>
     <t>IPB-2006ES-RN002-ST1-VE001</t>
   </si>
   <si>
@@ -3419,6 +3387,45 @@
   </si>
   <si>
     <t>Kumbang</t>
+  </si>
+  <si>
+    <t>IPB-2000WN-RN001-SCIKh-VE006</t>
+  </si>
+  <si>
+    <t>IPB-2000WN-RN001-SCIKh-VE001</t>
+  </si>
+  <si>
+    <t>IPB-2000WN-RN001-SCIKh-VE002</t>
+  </si>
+  <si>
+    <t>IPB-2000WN-RN001-SCIKh-VE003</t>
+  </si>
+  <si>
+    <t>IPB-2000WN-RN001-SCIKh-VE004</t>
+  </si>
+  <si>
+    <t>IPB-2000WN-RN001-SCIKh-VE005</t>
+  </si>
+  <si>
+    <t>IPB-2000WN-RN001-SCISh-VE001</t>
+  </si>
+  <si>
+    <t>IPB-2000WN-RN001-SCISh-VE002</t>
+  </si>
+  <si>
+    <t>IPB-2000WN-RN001-SCISh-VE003</t>
+  </si>
+  <si>
+    <t>IPB-2000WN-RN001-SCISh-VE004</t>
+  </si>
+  <si>
+    <t>IPB-2000WN-RN001-SCISh-VE005</t>
+  </si>
+  <si>
+    <t>IPB-2000WN-RN001-SCISh-VE006</t>
+  </si>
+  <si>
+    <t>IPB-2000WN-RN001-SCISh-VE007</t>
   </si>
 </sst>
 </file>
@@ -4172,30 +4179,30 @@
       <selection pane="bottomLeft" activeCell="T12" sqref="T12:T14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="18.58203125" style="14" customWidth="1"/>
     <col min="2" max="2" width="24.25" style="14" customWidth="1"/>
-    <col min="3" max="3" width="21.125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="20.125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="21.08203125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="20.08203125" style="14" customWidth="1"/>
     <col min="5" max="5" width="18" style="14" customWidth="1"/>
     <col min="6" max="6" width="17" style="14" customWidth="1"/>
-    <col min="7" max="7" width="17.625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="17.58203125" style="14" customWidth="1"/>
     <col min="8" max="8" width="13" style="14" customWidth="1"/>
-    <col min="9" max="10" width="14.875" style="14" customWidth="1"/>
-    <col min="11" max="11" width="17.625" style="15" customWidth="1"/>
+    <col min="9" max="10" width="14.83203125" style="14" customWidth="1"/>
+    <col min="11" max="11" width="17.58203125" style="15" customWidth="1"/>
     <col min="12" max="12" width="16.5" style="15" customWidth="1"/>
-    <col min="13" max="13" width="16.125" style="14" customWidth="1"/>
+    <col min="13" max="13" width="16.08203125" style="14" customWidth="1"/>
     <col min="14" max="16" width="13.5" style="14" customWidth="1"/>
     <col min="17" max="17" width="22.5" style="14" customWidth="1"/>
     <col min="18" max="18" width="20" style="14" customWidth="1"/>
-    <col min="19" max="19" width="31.625" style="14" customWidth="1"/>
+    <col min="19" max="19" width="31.58203125" style="14" customWidth="1"/>
     <col min="20" max="20" width="21.5" customWidth="1"/>
     <col min="21" max="21" width="54.5" style="14" customWidth="1"/>
     <col min="22" max="16384" width="11" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -4260,7 +4267,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>44</v>
       </c>
@@ -4325,7 +4332,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>44</v>
       </c>
@@ -4390,7 +4397,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>44</v>
       </c>
@@ -4455,7 +4462,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>44</v>
       </c>
@@ -4520,7 +4527,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>94</v>
       </c>
@@ -4579,13 +4586,13 @@
         <v>184</v>
       </c>
       <c r="T6" s="21" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="U6" s="14" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>94</v>
       </c>
@@ -4644,13 +4651,13 @@
         <v>203</v>
       </c>
       <c r="T7" s="21" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="U7" s="14" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>94</v>
       </c>
@@ -4709,13 +4716,13 @@
         <v>204</v>
       </c>
       <c r="T8" s="21" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="U8" s="14" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>94</v>
       </c>
@@ -4774,13 +4781,13 @@
         <v>205</v>
       </c>
       <c r="T9" s="21" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="U9" s="14" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>94</v>
       </c>
@@ -4839,13 +4846,13 @@
         <v>206</v>
       </c>
       <c r="T10" s="21" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="U10" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>119</v>
       </c>
@@ -4910,7 +4917,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>119</v>
       </c>
@@ -4969,13 +4976,13 @@
         <v>211</v>
       </c>
       <c r="T12" s="21" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="U12" s="14" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>119</v>
       </c>
@@ -5034,13 +5041,13 @@
         <v>213</v>
       </c>
       <c r="T13" s="21" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="U13" s="14" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
         <v>119</v>
       </c>
@@ -5099,7 +5106,7 @@
         <v>215</v>
       </c>
       <c r="T14" s="21" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="U14" s="14" t="s">
         <v>149</v>
@@ -5121,32 +5128,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q92"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H82" sqref="H82"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.875" customWidth="1"/>
-    <col min="2" max="2" width="28.375" customWidth="1"/>
-    <col min="3" max="3" width="18.625" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="33.4140625" customWidth="1"/>
+    <col min="3" max="3" width="18.58203125" customWidth="1"/>
     <col min="4" max="4" width="20.25" style="8" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
-    <col min="6" max="6" width="24.125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24.08203125" style="9" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.875" style="10" customWidth="1"/>
-    <col min="10" max="10" width="18.625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="15.625" customWidth="1"/>
+    <col min="8" max="8" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="18.58203125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="15.58203125" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="18.875" customWidth="1"/>
-    <col min="14" max="14" width="17.875" customWidth="1"/>
-    <col min="15" max="15" width="24.125" customWidth="1"/>
+    <col min="13" max="13" width="18.83203125" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" customWidth="1"/>
+    <col min="15" max="15" width="24.08203125" customWidth="1"/>
     <col min="16" max="16" width="21.5" customWidth="1"/>
     <col min="17" max="17" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -5199,7 +5206,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>70</v>
       </c>
@@ -5249,7 +5256,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>70</v>
       </c>
@@ -5299,7 +5306,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>70</v>
       </c>
@@ -5349,7 +5356,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>70</v>
       </c>
@@ -5399,7 +5406,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>70</v>
       </c>
@@ -5449,12 +5456,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>71</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>225</v>
+        <v>310</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>145</v>
@@ -5499,12 +5506,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>71</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>226</v>
+        <v>311</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>145</v>
@@ -5549,12 +5556,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>71</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>227</v>
+        <v>312</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>145</v>
@@ -5599,12 +5606,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>71</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>228</v>
+        <v>313</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>145</v>
@@ -5649,12 +5656,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>71</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>229</v>
+        <v>314</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>145</v>
@@ -5699,12 +5706,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>71</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>230</v>
+        <v>309</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>145</v>
@@ -5749,12 +5756,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>75</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>145</v>
@@ -5799,12 +5806,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>75</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>145</v>
@@ -5849,12 +5856,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>75</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>145</v>
@@ -5899,12 +5906,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>75</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>145</v>
@@ -5949,12 +5956,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>76</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>231</v>
+        <v>315</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>145</v>
@@ -5999,12 +6006,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>76</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>232</v>
+        <v>316</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>145</v>
@@ -6049,12 +6056,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>76</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>233</v>
+        <v>317</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>145</v>
@@ -6099,12 +6106,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
         <v>76</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>234</v>
+        <v>318</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>145</v>
@@ -6149,12 +6156,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
         <v>76</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>235</v>
+        <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>145</v>
@@ -6199,12 +6206,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="s">
         <v>76</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>236</v>
+        <v>320</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>145</v>
@@ -6249,12 +6256,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="14" t="s">
         <v>76</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>237</v>
+        <v>321</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>145</v>
@@ -6299,12 +6306,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="14" t="s">
         <v>187</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>145</v>
@@ -6349,12 +6356,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14" t="s">
         <v>187</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>145</v>
@@ -6399,12 +6406,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14" t="s">
         <v>187</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>145</v>
@@ -6449,12 +6456,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="s">
         <v>187</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>145</v>
@@ -6499,12 +6506,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="s">
         <v>187</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>145</v>
@@ -6549,12 +6556,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="14" t="s">
         <v>183</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>145</v>
@@ -6599,12 +6606,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="s">
         <v>183</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>145</v>
@@ -6649,12 +6656,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
         <v>183</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>145</v>
@@ -6699,12 +6706,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
         <v>183</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>145</v>
@@ -6749,12 +6756,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="14" t="s">
         <v>183</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>145</v>
@@ -6799,12 +6806,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
         <v>183</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>145</v>
@@ -6849,12 +6856,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="14" t="s">
         <v>180</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>145</v>
@@ -6899,12 +6906,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="14" t="s">
         <v>180</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>145</v>
@@ -6949,12 +6956,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
         <v>180</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>145</v>
@@ -6999,12 +7006,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="14" t="s">
         <v>180</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>145</v>
@@ -7049,12 +7056,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="14" t="s">
         <v>180</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>145</v>
@@ -7099,12 +7106,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="14" t="s">
         <v>180</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>145</v>
@@ -7149,12 +7156,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="14" t="s">
         <v>180</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>145</v>
@@ -7199,12 +7206,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="14" t="s">
         <v>177</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>145</v>
@@ -7249,12 +7256,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="14" t="s">
         <v>177</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>145</v>
@@ -7299,12 +7306,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="14" t="s">
         <v>177</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>145</v>
@@ -7349,12 +7356,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="14" t="s">
         <v>177</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>145</v>
@@ -7399,12 +7406,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="14" t="s">
         <v>177</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>145</v>
@@ -7449,12 +7456,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="14" t="s">
         <v>177</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>145</v>
@@ -7499,12 +7506,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="14" t="s">
         <v>177</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>145</v>
@@ -7549,12 +7556,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="49" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="14" t="s">
         <v>177</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C49" s="14" t="s">
         <v>145</v>
@@ -7599,12 +7606,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
         <v>174</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C50" s="14" t="s">
         <v>145</v>
@@ -7649,12 +7656,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="14" t="s">
         <v>174</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C51" s="14" t="s">
         <v>145</v>
@@ -7699,12 +7706,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="52" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="14" t="s">
         <v>174</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>145</v>
@@ -7749,12 +7756,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="53" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="14" t="s">
         <v>174</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C53" s="14" t="s">
         <v>145</v>
@@ -7799,12 +7806,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="54" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="14" t="s">
         <v>174</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C54" s="14" t="s">
         <v>145</v>
@@ -7849,12 +7856,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="55" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="14" t="s">
         <v>174</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C55" s="14" t="s">
         <v>145</v>
@@ -7899,12 +7906,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="56" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="14" t="s">
         <v>174</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>145</v>
@@ -7949,12 +7956,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="57" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="14" t="s">
         <v>174</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C57" s="14" t="s">
         <v>145</v>
@@ -7999,12 +8006,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="58" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="14" t="s">
         <v>174</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C58" s="14" t="s">
         <v>145</v>
@@ -8049,12 +8056,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="59" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="18" t="s">
         <v>169</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C59" s="14" t="s">
         <v>145</v>
@@ -8072,7 +8079,7 @@
         <v>63</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="I59" s="20" t="s">
         <v>167</v>
@@ -8099,12 +8106,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="18" t="s">
         <v>169</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>145</v>
@@ -8122,7 +8129,7 @@
         <v>63</v>
       </c>
       <c r="H60" s="14" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="I60" s="20" t="s">
         <v>167</v>
@@ -8149,12 +8156,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="61" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="18" t="s">
         <v>169</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>145</v>
@@ -8172,7 +8179,7 @@
         <v>63</v>
       </c>
       <c r="H61" s="14" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="I61" s="20" t="s">
         <v>167</v>
@@ -8202,12 +8209,12 @@
         <v>140</v>
       </c>
     </row>
-    <row r="62" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="18" t="s">
         <v>169</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>145</v>
@@ -8225,7 +8232,7 @@
         <v>63</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="I62" s="20" t="s">
         <v>167</v>
@@ -8255,12 +8262,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="18" t="s">
         <v>169</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C63" s="14" t="s">
         <v>145</v>
@@ -8278,7 +8285,7 @@
         <v>63</v>
       </c>
       <c r="H63" s="14" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="I63" s="20" t="s">
         <v>167</v>
@@ -8308,12 +8315,12 @@
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="18" t="s">
         <v>169</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C64" s="14" t="s">
         <v>145</v>
@@ -8331,7 +8338,7 @@
         <v>63</v>
       </c>
       <c r="H64" s="14" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="I64" s="20" t="s">
         <v>167</v>
@@ -8358,12 +8365,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="18" t="s">
         <v>169</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="C65" s="14" t="s">
         <v>145</v>
@@ -8381,7 +8388,7 @@
         <v>63</v>
       </c>
       <c r="H65" s="14" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="I65" s="20" t="s">
         <v>167</v>
@@ -8408,12 +8415,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="18" t="s">
         <v>165</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="C66" s="14" t="s">
         <v>145</v>
@@ -8431,7 +8438,7 @@
         <v>63</v>
       </c>
       <c r="H66" s="14" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="I66" s="20" t="s">
         <v>163</v>
@@ -8458,12 +8465,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="67" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="18" t="s">
         <v>165</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>145</v>
@@ -8481,7 +8488,7 @@
         <v>63</v>
       </c>
       <c r="H67" s="14" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="I67" s="20" t="s">
         <v>163</v>
@@ -8508,12 +8515,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="18" t="s">
         <v>165</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>145</v>
@@ -8531,7 +8538,7 @@
         <v>63</v>
       </c>
       <c r="H68" s="14" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="I68" s="20" t="s">
         <v>163</v>
@@ -8558,12 +8565,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="18" t="s">
         <v>165</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="C69" s="14" t="s">
         <v>145</v>
@@ -8581,7 +8588,7 @@
         <v>63</v>
       </c>
       <c r="H69" s="14" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="I69" s="20" t="s">
         <v>163</v>
@@ -8608,12 +8615,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="70" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="18" t="s">
         <v>165</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C70" s="14" t="s">
         <v>145</v>
@@ -8631,7 +8638,7 @@
         <v>63</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="I70" s="20" t="s">
         <v>163</v>
@@ -8658,12 +8665,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="71" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="18" t="s">
         <v>165</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="C71" s="14" t="s">
         <v>145</v>
@@ -8681,7 +8688,7 @@
         <v>58</v>
       </c>
       <c r="H71" s="14" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="I71" s="20" t="s">
         <v>163</v>
@@ -8708,12 +8715,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="72" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="18" t="s">
         <v>165</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="C72" s="14" t="s">
         <v>145</v>
@@ -8731,7 +8738,7 @@
         <v>58</v>
       </c>
       <c r="H72" s="14" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="I72" s="20" t="s">
         <v>163</v>
@@ -8758,12 +8765,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="73" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="18" t="s">
         <v>161</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>145</v>
@@ -8781,7 +8788,7 @@
         <v>63</v>
       </c>
       <c r="H73" s="14" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="I73" s="20" t="s">
         <v>159</v>
@@ -8808,12 +8815,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="74" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="18" t="s">
         <v>161</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="C74" s="14" t="s">
         <v>145</v>
@@ -8831,7 +8838,7 @@
         <v>63</v>
       </c>
       <c r="H74" s="14" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="I74" s="20" t="s">
         <v>159</v>
@@ -8858,12 +8865,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="75" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="18" t="s">
         <v>161</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>145</v>
@@ -8881,7 +8888,7 @@
         <v>63</v>
       </c>
       <c r="H75" s="14" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="I75" s="20" t="s">
         <v>159</v>
@@ -8908,12 +8915,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="76" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="18" t="s">
         <v>161</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="C76" s="14" t="s">
         <v>145</v>
@@ -8931,7 +8938,7 @@
         <v>63</v>
       </c>
       <c r="H76" s="14" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="I76" s="20" t="s">
         <v>159</v>
@@ -8958,12 +8965,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="77" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="18" t="s">
         <v>161</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C77" s="14" t="s">
         <v>145</v>
@@ -8981,7 +8988,7 @@
         <v>63</v>
       </c>
       <c r="H77" s="14" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="I77" s="20" t="s">
         <v>159</v>
@@ -9008,12 +9015,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="18" t="s">
         <v>161</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="C78" s="14" t="s">
         <v>145</v>
@@ -9031,7 +9038,7 @@
         <v>58</v>
       </c>
       <c r="H78" s="14" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="I78" s="20" t="s">
         <v>159</v>
@@ -9058,12 +9065,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="79" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="18" t="s">
         <v>161</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="C79" s="14" t="s">
         <v>145</v>
@@ -9081,7 +9088,7 @@
         <v>58</v>
       </c>
       <c r="H79" s="14" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="I79" s="20" t="s">
         <v>159</v>
@@ -9108,12 +9115,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="80" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80" s="18" t="s">
         <v>161</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C80" s="14" t="s">
         <v>145</v>
@@ -9131,7 +9138,7 @@
         <v>58</v>
       </c>
       <c r="H80" s="14" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="I80" s="20" t="s">
         <v>159</v>
@@ -9158,12 +9165,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="81" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A81" s="18" t="s">
         <v>161</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C81" s="14" t="s">
         <v>145</v>
@@ -9181,7 +9188,7 @@
         <v>58</v>
       </c>
       <c r="H81" s="14" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="I81" s="20" t="s">
         <v>159</v>
@@ -9208,12 +9215,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="82" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="18" t="s">
         <v>157</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="C82" s="14" t="s">
         <v>145</v>
@@ -9231,7 +9238,7 @@
         <v>63</v>
       </c>
       <c r="H82" s="14" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="I82" s="20" t="s">
         <v>152</v>
@@ -9258,12 +9265,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="83" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A83" s="18" t="s">
         <v>157</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="C83" s="14" t="s">
         <v>145</v>
@@ -9281,7 +9288,7 @@
         <v>63</v>
       </c>
       <c r="H83" s="14" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="I83" s="20" t="s">
         <v>152</v>
@@ -9308,12 +9315,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="84" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A84" s="18" t="s">
         <v>157</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C84" s="14" t="s">
         <v>145</v>
@@ -9331,7 +9338,7 @@
         <v>63</v>
       </c>
       <c r="H84" s="14" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="I84" s="20" t="s">
         <v>152</v>
@@ -9358,12 +9365,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="85" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A85" s="18" t="s">
         <v>157</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C85" s="14" t="s">
         <v>145</v>
@@ -9381,7 +9388,7 @@
         <v>63</v>
       </c>
       <c r="H85" s="14" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="I85" s="20" t="s">
         <v>152</v>
@@ -9408,12 +9415,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="86" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A86" s="18" t="s">
         <v>157</v>
       </c>
       <c r="B86" s="18" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C86" s="14" t="s">
         <v>145</v>
@@ -9431,7 +9438,7 @@
         <v>63</v>
       </c>
       <c r="H86" s="14" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="I86" s="20" t="s">
         <v>152</v>
@@ -9458,12 +9465,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="87" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="18" t="s">
         <v>157</v>
       </c>
       <c r="B87" s="18" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="C87" s="14" t="s">
         <v>145</v>
@@ -9481,7 +9488,7 @@
         <v>58</v>
       </c>
       <c r="H87" s="14" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="I87" s="20" t="s">
         <v>152</v>
@@ -9508,12 +9515,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="88" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="18" t="s">
         <v>157</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>145</v>
@@ -9531,7 +9538,7 @@
         <v>58</v>
       </c>
       <c r="H88" s="14" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="I88" s="20" t="s">
         <v>152</v>
@@ -9558,12 +9565,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="89" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A89" s="18" t="s">
         <v>157</v>
       </c>
       <c r="B89" s="18" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="C89" s="14" t="s">
         <v>145</v>
@@ -9581,7 +9588,7 @@
         <v>58</v>
       </c>
       <c r="H89" s="14" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="I89" s="20" t="s">
         <v>152</v>
@@ -9608,12 +9615,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="90" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="18" t="s">
         <v>157</v>
       </c>
       <c r="B90" s="18" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C90" s="14" t="s">
         <v>145</v>
@@ -9631,7 +9638,7 @@
         <v>58</v>
       </c>
       <c r="H90" s="14" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="I90" s="20" t="s">
         <v>152</v>
@@ -9658,12 +9665,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="91" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="18" t="s">
         <v>157</v>
       </c>
       <c r="B91" s="18" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="C91" s="14" t="s">
         <v>145</v>
@@ -9681,7 +9688,7 @@
         <v>58</v>
       </c>
       <c r="H91" s="14" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="I91" s="20" t="s">
         <v>152</v>
@@ -9708,12 +9715,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="92" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A92" s="18" t="s">
         <v>157</v>
       </c>
       <c r="B92" s="18" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C92" s="14" t="s">
         <v>145</v>
@@ -9731,7 +9738,7 @@
         <v>58</v>
       </c>
       <c r="H92" s="14" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="I92" s="20" t="s">
         <v>152</v>
@@ -9779,20 +9786,20 @@
       <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="44.125" customWidth="1"/>
+    <col min="2" max="2" width="44.08203125" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="15.625" customWidth="1"/>
-    <col min="7" max="7" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="15.58203125" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
     <col min="8" max="8" width="34.5" customWidth="1"/>
     <col min="9" max="9" width="19.25" customWidth="1"/>
-    <col min="10" max="10" width="39.375" customWidth="1"/>
+    <col min="10" max="10" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -9824,7 +9831,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -9856,7 +9863,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>94</v>
       </c>
@@ -9888,7 +9895,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>119</v>
       </c>
@@ -9917,11 +9924,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
     </row>
@@ -9941,24 +9948,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.75" customWidth="1"/>
     <col min="4" max="4" width="15.25" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="21.75" customWidth="1"/>
     <col min="7" max="7" width="19.75" customWidth="1"/>
-    <col min="8" max="8" width="28.625" customWidth="1"/>
-    <col min="9" max="9" width="22.625" customWidth="1"/>
+    <col min="8" max="8" width="28.58203125" customWidth="1"/>
+    <col min="9" max="9" width="22.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>